<commit_message>
Funcionalidad eliminar object de S3
</commit_message>
<xml_diff>
--- a/Backend/controllers/excel/ReporteSemanalGersa.xlsx
+++ b/Backend/controllers/excel/ReporteSemanalGersa.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Reporte empleados Periodo:2022-05-02 a 2022-05-02</t>
   </si>
@@ -55,7 +55,7 @@
     <t>Fin Hora Extra</t>
   </si>
   <si>
-    <t/>
+    <t>1001</t>
   </si>
   <si>
     <t>Admin Master</t>
@@ -64,7 +64,7 @@
     <t>No tiene registro</t>
   </si>
   <si>
-    <t>333385</t>
+    <t>1002</t>
   </si>
   <si>
     <t>Ivan Santana Santana</t>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>2022-05-08</t>
+  </si>
+  <si>
+    <t>1003</t>
+  </si>
+  <si>
+    <t>Ivan Arrieta Arrieta</t>
   </si>
 </sst>
 </file>
@@ -554,10 +560,10 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>16</v>

</xml_diff>